<commit_message>
[Bug] Fixed not appending of excel
</commit_message>
<xml_diff>
--- a/R-package/data/test-data/quick-test/ODM_dictionary_9.9.9.xlsx
+++ b/R-package/data/test-data/quick-test/ODM_dictionary_9.9.9.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -52,7 +52,7 @@
     <t>Should fail since trying to record a set as csv</t>
   </si>
   <si>
-    <t>CSV_FAIL</t>
+    <t>CSV_PASS</t>
   </si>
   <si>
     <t>csv</t>
@@ -76,13 +76,13 @@
     <t>Should fail since trying to record excel with not a set</t>
   </si>
   <si>
-    <t>EXCEL_FAIL</t>
+    <t>EXCEL_PASS</t>
   </si>
   <si>
     <t>excel</t>
   </si>
   <si>
-    <t>DoesntExistInSets</t>
+    <t>ExistInSets</t>
   </si>
   <si>
     <t>version</t>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>ExistInSets</t>
   </si>
   <si>
     <t>tester</t>
@@ -1180,19 +1177,19 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>84</v>
@@ -1201,10 +1198,10 @@
         <v>84</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1224,10 +1221,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1247,10 +1244,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1270,10 +1267,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1293,10 +1290,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>